<commit_message>
request format and download alert added
</commit_message>
<xml_diff>
--- a/my_selected_milestones.xlsx
+++ b/my_selected_milestones.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Milestone 4</t>
+          <t>Milestone 2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,18 +460,10 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Milestone 5</t>
+          <t>Milestone 4</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Milestone 6</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
request clean-up and ReadMe change
</commit_message>
<xml_diff>
--- a/my_selected_milestones.xlsx
+++ b/my_selected_milestones.xlsx
@@ -448,12 +448,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Milestone 2</t>
+          <t>Milestone 3</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2022-03-15</t>
+          <t>2022-05-15</t>
         </is>
       </c>
     </row>

</xml_diff>